<commit_message>
WebAppData updates to policy descriptions
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-canada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E19869-D415-460B-886A-772398E3F795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7DB5F-002D-4D19-B9B1-C9BEC06A2FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="9765" tabRatio="832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12450" yWindow="-16470" windowWidth="29340" windowHeight="16140" tabRatio="832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5486" uniqueCount="1231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5486" uniqueCount="1232">
   <si>
     <t>Short Name</t>
   </si>
@@ -4169,9 +4169,6 @@
     <t>**Description:** This policy reduces the subsidies paid for the production of the selected energy source(s) in the BAU case. // **Guidance for setting values:** A value of 100% eliminates subsidies, increasing the price of coal by 8% (varying by sector), natural gas by 3-8% (varying by sector), petroleum gasoline by 1%, petroleum diesel by 2% (varying by sector) in 2050, and jet fuel by 2% (varying by sector) in 2050.</t>
   </si>
   <si>
-    <t>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</t>
-  </si>
-  <si>
     <t>**Description:** This policy reduces fuel consumption by the selected industry by increasing the efficiency of industrial equipment through stronger standards.  The policy setting refers to overall energy use reduction, not the reduction in energy use of newly sold equipment. // **Guidance for setting values:** In 2016, the U.S. Department of Energy developed an industrial energy efficiency potential analysis that suggests a potential improvement rate of 2.4% per year through 2030, instead of a BAU rate of 1.2% per year.  Extended through 2050, this equates to a maximum potential improvement of 33% by 2050 relative to BAU.  The same potential may exist in Canada.</t>
   </si>
   <si>
@@ -4215,6 +4212,12 @@
   </si>
   <si>
     <t>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</t>
+  </si>
+  <si>
+    <t>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</t>
+  </si>
+  <si>
+    <t>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</t>
   </si>
 </sst>
 </file>
@@ -5409,6 +5412,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5417,9 +5423,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6512,8 +6515,8 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6530,7 +6533,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" s="189" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B1" s="187"/>
       <c r="C1" s="187"/>
@@ -6548,7 +6551,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="188" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B2" s="187"/>
       <c r="C2" s="187"/>
@@ -6608,7 +6611,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:14" ht="100.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -6637,7 +6640,7 @@
         <v>1090</v>
       </c>
       <c r="J4" s="169" t="s">
-        <v>1091</v>
+        <v>1230</v>
       </c>
       <c r="K4" s="76" t="s">
         <v>1092</v>
@@ -6713,7 +6716,7 @@
         <v>579</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="K6" s="76" t="s">
         <v>580</v>
@@ -6833,7 +6836,7 @@
         <v>128</v>
       </c>
       <c r="J9" s="169" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="K9" s="169" t="s">
         <v>237</v>
@@ -6911,7 +6914,7 @@
         <v>43</v>
       </c>
       <c r="J11" s="169" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="K11" s="169" t="s">
         <v>239</v>
@@ -6952,7 +6955,7 @@
         <v>130</v>
       </c>
       <c r="J12" s="169" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="K12" s="169" t="s">
         <v>241</v>
@@ -6990,7 +6993,7 @@
         <v>37</v>
       </c>
       <c r="J13" s="169" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K13" s="169" t="s">
         <v>243</v>
@@ -7194,7 +7197,7 @@
         <v>42</v>
       </c>
       <c r="J18" s="169" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K18" s="169" t="s">
         <v>249</v>
@@ -7238,7 +7241,7 @@
         <v>34</v>
       </c>
       <c r="J19" s="169" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K19" s="169" t="s">
         <v>251</v>
@@ -7276,7 +7279,7 @@
         <v>34</v>
       </c>
       <c r="J20" s="169" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="K20" s="169" t="s">
         <v>414</v>
@@ -7462,7 +7465,7 @@
         <v>231</v>
       </c>
       <c r="J25" s="169" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K25" s="169" t="s">
         <v>255</v>
@@ -7696,7 +7699,7 @@
         <v>313</v>
       </c>
       <c r="J31" s="169" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K31" s="168" t="s">
         <v>612</v>
@@ -7736,7 +7739,7 @@
         <v>815</v>
       </c>
       <c r="J32" s="169" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="K32" s="168" t="s">
         <v>942</v>
@@ -7852,7 +7855,7 @@
         <v>994</v>
       </c>
       <c r="J35" s="169" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K35" s="169" t="s">
         <v>263</v>
@@ -8017,7 +8020,7 @@
         <v>37</v>
       </c>
       <c r="J39" s="169" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="K39" s="169" t="s">
         <v>271</v>
@@ -8792,7 +8795,7 @@
       </c>
       <c r="N58" s="169"/>
     </row>
-    <row r="59" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:14" ht="140.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A59" s="169" t="s">
         <v>10</v>
       </c>
@@ -8821,7 +8824,7 @@
         <v>1014</v>
       </c>
       <c r="J59" s="169" t="s">
-        <v>1215</v>
+        <v>1231</v>
       </c>
       <c r="K59" s="169" t="s">
         <v>295</v>
@@ -9496,7 +9499,7 @@
       </c>
       <c r="P2" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C2,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q2" s="76" t="s">
         <v>1092</v>
@@ -9558,7 +9561,7 @@
       </c>
       <c r="P3" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C3,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q3" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9622,7 +9625,7 @@
       </c>
       <c r="P4" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C4,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q4" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9686,7 +9689,7 @@
       </c>
       <c r="P5" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C5,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q5" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9750,7 +9753,7 @@
       </c>
       <c r="P6" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C6,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q6" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9814,7 +9817,7 @@
       </c>
       <c r="P7" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C7,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q7" s="166" t="str">
         <f t="shared" si="1"/>
@@ -21955,7 +21958,7 @@
       </c>
       <c r="P225" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C225,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q225" s="56" t="s">
         <v>295</v>
@@ -22023,7 +22026,7 @@
       </c>
       <c r="P226" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C226,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q226" s="58" t="str">
         <f t="shared" ref="Q226:R229" si="45">Q$225</f>
@@ -22089,7 +22092,7 @@
       </c>
       <c r="P227" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C227,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q227" s="58" t="str">
         <f t="shared" si="45"/>
@@ -22155,7 +22158,7 @@
       </c>
       <c r="P228" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C228,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q228" s="58" t="str">
         <f t="shared" si="45"/>
@@ -22221,7 +22224,7 @@
       </c>
       <c r="P229" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C229,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q229" s="58" t="str">
         <f t="shared" si="45"/>
@@ -22273,7 +22276,7 @@
       <c r="O230" s="56"/>
       <c r="P230" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C230,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q230" s="56"/>
       <c r="R230" s="11"/>
@@ -22319,7 +22322,7 @@
       <c r="O231" s="56"/>
       <c r="P231" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C231,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q231" s="56"/>
       <c r="R231" s="11"/>
@@ -31994,13 +31997,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="195" t="s">
+      <c r="A1" s="192" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="195"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="196" t="s">
@@ -32069,13 +32072,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" s="195" t="s">
+      <c r="A60" s="192" t="s">
         <v>200</v>
       </c>
-      <c r="B60" s="195"/>
-      <c r="C60" s="195"/>
-      <c r="D60" s="195"/>
-      <c r="E60" s="195"/>
+      <c r="B60" s="192"/>
+      <c r="C60" s="192"/>
+      <c r="D60" s="192"/>
+      <c r="E60" s="192"/>
     </row>
     <row r="85" spans="1:39" s="13" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="10" t="s">
@@ -32180,13 +32183,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.75">
-      <c r="A89" s="195" t="s">
+      <c r="A89" s="192" t="s">
         <v>201</v>
       </c>
-      <c r="B89" s="195"/>
-      <c r="C89" s="195"/>
-      <c r="D89" s="195"/>
-      <c r="E89" s="195"/>
+      <c r="B89" s="192"/>
+      <c r="C89" s="192"/>
+      <c r="D89" s="192"/>
+      <c r="E89" s="192"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.75">
       <c r="A90" s="10">
@@ -32273,13 +32276,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A98" s="195" t="s">
+      <c r="A98" s="192" t="s">
         <v>202</v>
       </c>
-      <c r="B98" s="195"/>
-      <c r="C98" s="195"/>
-      <c r="D98" s="195"/>
-      <c r="E98" s="195"/>
+      <c r="B98" s="192"/>
+      <c r="C98" s="192"/>
+      <c r="D98" s="192"/>
+      <c r="E98" s="192"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" s="18">
@@ -32363,13 +32366,13 @@
       <c r="A108" s="21"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A109" s="195" t="s">
+      <c r="A109" s="192" t="s">
         <v>204</v>
       </c>
-      <c r="B109" s="195"/>
-      <c r="C109" s="195"/>
-      <c r="D109" s="195"/>
-      <c r="E109" s="195"/>
+      <c r="B109" s="192"/>
+      <c r="C109" s="192"/>
+      <c r="D109" s="192"/>
+      <c r="E109" s="192"/>
     </row>
     <row r="110" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="111" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -32382,13 +32385,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A113" s="195" t="s">
+      <c r="A113" s="192" t="s">
         <v>203</v>
       </c>
-      <c r="B113" s="195"/>
-      <c r="C113" s="195"/>
-      <c r="D113" s="195"/>
-      <c r="E113" s="195"/>
+      <c r="B113" s="192"/>
+      <c r="C113" s="192"/>
+      <c r="D113" s="192"/>
+      <c r="E113" s="192"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A114" s="18">
@@ -32469,13 +32472,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A124" s="195" t="s">
+      <c r="A124" s="192" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="195"/>
-      <c r="C124" s="195"/>
-      <c r="D124" s="195"/>
-      <c r="E124" s="195"/>
+      <c r="B124" s="192"/>
+      <c r="C124" s="192"/>
+      <c r="D124" s="192"/>
+      <c r="E124" s="192"/>
       <c r="L124" s="22"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.75">
@@ -32566,13 +32569,13 @@
       <c r="C133" s="16"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A134" s="195" t="s">
+      <c r="A134" s="192" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="195"/>
-      <c r="C134" s="195"/>
-      <c r="D134" s="195"/>
-      <c r="E134" s="195"/>
+      <c r="B134" s="192"/>
+      <c r="C134" s="192"/>
+      <c r="D134" s="192"/>
+      <c r="E134" s="192"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A135" s="28" t="s">
@@ -32587,25 +32590,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A136" s="30"/>
-      <c r="B136" s="192" t="s">
+      <c r="B136" s="193" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="193"/>
-      <c r="D136" s="193"/>
-      <c r="E136" s="194"/>
+      <c r="C136" s="194"/>
+      <c r="D136" s="194"/>
+      <c r="E136" s="195"/>
       <c r="F136" s="29"/>
       <c r="G136" s="29"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A137" s="31"/>
-      <c r="B137" s="192" t="s">
+      <c r="B137" s="193" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="194"/>
-      <c r="D137" s="192" t="s">
+      <c r="C137" s="195"/>
+      <c r="D137" s="193" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="194"/>
+      <c r="E137" s="195"/>
       <c r="F137" s="29"/>
       <c r="G137" s="29"/>
     </row>
@@ -33152,13 +33155,13 @@
       <c r="G163" s="29"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A165" s="195" t="s">
+      <c r="A165" s="192" t="s">
         <v>207</v>
       </c>
-      <c r="B165" s="195"/>
-      <c r="C165" s="195"/>
-      <c r="D165" s="195"/>
-      <c r="E165" s="195"/>
+      <c r="B165" s="192"/>
+      <c r="C165" s="192"/>
+      <c r="D165" s="192"/>
+      <c r="E165" s="192"/>
     </row>
     <row r="166" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A166" s="24" t="s">
@@ -33181,10 +33184,10 @@
       <c r="B168" s="47"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A169" s="195" t="s">
+      <c r="A169" s="192" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="195"/>
+      <c r="B169" s="192"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" s="24" t="s">
@@ -33216,13 +33219,13 @@
       <c r="B173" s="47"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A174" s="195" t="s">
+      <c r="A174" s="192" t="s">
         <v>217</v>
       </c>
-      <c r="B174" s="195"/>
-      <c r="C174" s="195"/>
-      <c r="D174" s="195"/>
-      <c r="E174" s="195"/>
+      <c r="B174" s="192"/>
+      <c r="C174" s="192"/>
+      <c r="D174" s="192"/>
+      <c r="E174" s="192"/>
     </row>
     <row r="175" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A175" s="24" t="s">
@@ -33242,13 +33245,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A178" s="195" t="s">
+      <c r="A178" s="192" t="s">
         <v>210</v>
       </c>
-      <c r="B178" s="195"/>
-      <c r="C178" s="195"/>
-      <c r="D178" s="195"/>
-      <c r="E178" s="195"/>
+      <c r="B178" s="192"/>
+      <c r="C178" s="192"/>
+      <c r="D178" s="192"/>
+      <c r="E178" s="192"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" s="26" t="s">
@@ -33276,13 +33279,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A183" s="195" t="s">
+      <c r="A183" s="192" t="s">
         <v>212</v>
       </c>
-      <c r="B183" s="195"/>
-      <c r="C183" s="195"/>
-      <c r="D183" s="195"/>
-      <c r="E183" s="195"/>
+      <c r="B183" s="192"/>
+      <c r="C183" s="192"/>
+      <c r="D183" s="192"/>
+      <c r="E183" s="192"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" s="24" t="s">
@@ -33337,13 +33340,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A191" s="195" t="s">
+      <c r="A191" s="192" t="s">
         <v>228</v>
       </c>
-      <c r="B191" s="195"/>
-      <c r="C191" s="195"/>
-      <c r="D191" s="195"/>
-      <c r="E191" s="195"/>
+      <c r="B191" s="192"/>
+      <c r="C191" s="192"/>
+      <c r="D191" s="192"/>
+      <c r="E191" s="192"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" s="22" t="s">
@@ -33403,12 +33406,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -33423,6 +33420,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated descriptions to WebAppData file
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-canada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7DB5F-002D-4D19-B9B1-C9BEC06A2FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE6F391-A78F-4376-AE85-03C0E062EA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12450" yWindow="-16470" windowWidth="29340" windowHeight="16140" tabRatio="832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5486" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5486" uniqueCount="1233">
   <si>
     <t>Short Name</t>
   </si>
@@ -4196,9 +4196,6 @@
     <t>**Description:** This policy tightens energy efficiency standards for the selected component(s) in the selected building type(s).  The policy only applies to newly sold components each year (whether for new buildings or replacement of old components of existing buildings). // **Guidance for setting values:** In "Assessment of Electricity Savings in the U.S. Achievable through New Appliance/Equipment Efficiency Standards and Building Efficiency Codes, 2010-2025" (2011), the Edison Foundation considered a 30% reduction in whole-building energy use (moderate case) and 40-45% (aggressive case) relative to BAU from 2010 to 2025.  Similar potentials may be possible in Canada, with further improvement post-2025.</t>
   </si>
   <si>
-    <t>**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</t>
-  </si>
-  <si>
     <t xml:space="preserve">**Description:** Transportation Demand Management (TDM) represents a set of policies aimed at reducing demand for certain modes of travel. Passenger Transportation Demand Management (TDM) is aimed at reducing demand for passenger travel, especially in private automobiles.  These policies can include improved public transit systems, more walking and bike paths, zoning for higher density along transit corridors, zoning for mixed-use developments, roadway and congestion pricing, and increased parking fees.  Freight Transportation Demand Management (TDM) represents a set of policies aimed primarily at shifting freight from trucks to rail.  We use the International Energy Agency's BLUE Shifts scenario (from the 2009 report "Transport, Energy, and CO2: Moving Toward Sustainability") to represent passenger TDM policies as a whole. // **Guidance for setting values:** A value of "100%" fully implements the IEA's BLUE Shifts scenario by 2050, which is in line with IEA expectations (since their scenario assumes implementation by 2050). </t>
   </si>
   <si>
@@ -4214,10 +4211,16 @@
     <t>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</t>
   </si>
   <si>
-    <t>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</t>
-  </si>
-  <si>
     <t>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percentile estimate (in inflation-adjusted 2012 Canadian dollars).</t>
+  </si>
+  <si>
+    <t>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</t>
+  </si>
+  <si>
+    <t>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</t>
+  </si>
+  <si>
+    <t>**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</t>
   </si>
 </sst>
 </file>
@@ -5412,9 +5415,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5423,6 +5423,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6515,8 +6518,8 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6533,7 +6536,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" s="189" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B1" s="187"/>
       <c r="C1" s="187"/>
@@ -6551,7 +6554,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="188" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B2" s="187"/>
       <c r="C2" s="187"/>
@@ -6716,7 +6719,7 @@
         <v>579</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="K6" s="76" t="s">
         <v>580</v>
@@ -6754,7 +6757,7 @@
         <v>567</v>
       </c>
       <c r="J7" s="169" t="s">
-        <v>951</v>
+        <v>1231</v>
       </c>
       <c r="K7" s="76" t="s">
         <v>568</v>
@@ -6836,7 +6839,7 @@
         <v>128</v>
       </c>
       <c r="J9" s="169" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="K9" s="169" t="s">
         <v>237</v>
@@ -6914,7 +6917,7 @@
         <v>43</v>
       </c>
       <c r="J11" s="169" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="K11" s="169" t="s">
         <v>239</v>
@@ -6926,7 +6929,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="95.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:14" ht="128.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A12" s="169" t="s">
         <v>82</v>
       </c>
@@ -6955,7 +6958,7 @@
         <v>130</v>
       </c>
       <c r="J12" s="169" t="s">
-        <v>1224</v>
+        <v>1232</v>
       </c>
       <c r="K12" s="169" t="s">
         <v>241</v>
@@ -8824,7 +8827,7 @@
         <v>1014</v>
       </c>
       <c r="J59" s="169" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="K59" s="169" t="s">
         <v>295</v>
@@ -9367,8 +9370,8 @@
   <dimension ref="A1:T327"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K322" sqref="K322:O322"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9499,7 +9502,7 @@
       </c>
       <c r="P2" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C2,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q2" s="76" t="s">
         <v>1092</v>
@@ -9561,7 +9564,7 @@
       </c>
       <c r="P3" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C3,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q3" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9625,7 +9628,7 @@
       </c>
       <c r="P4" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C4,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q4" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9689,7 +9692,7 @@
       </c>
       <c r="P5" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C5,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q5" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9753,7 +9756,7 @@
       </c>
       <c r="P6" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C6,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q6" s="166" t="str">
         <f t="shared" si="1"/>
@@ -9817,7 +9820,7 @@
       </c>
       <c r="P7" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C7,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
+        <v>**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In the United States, since 1997, the 24-hour national ambient air quality standard (NAAQS) for PM2.5, the most harmful type of particulate for human health, declined from 65 µg/m^3 to 35 µg/m^3, a reduction of 46%.</v>
       </c>
       <c r="Q7" s="166" t="str">
         <f t="shared" si="1"/>
@@ -10616,7 +10619,7 @@
       </c>
       <c r="P21" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C21,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q21" s="76" t="s">
         <v>568</v>
@@ -10670,7 +10673,7 @@
       <c r="O22" s="78"/>
       <c r="P22" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C22,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q22" s="78"/>
       <c r="R22" s="78"/>
@@ -10720,7 +10723,7 @@
       <c r="O23" s="78"/>
       <c r="P23" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C23,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q23" s="78"/>
       <c r="R23" s="78"/>
@@ -10784,7 +10787,7 @@
       </c>
       <c r="P24" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C24,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q24" s="58" t="str">
         <f t="shared" si="8"/>
@@ -10840,7 +10843,7 @@
       <c r="O25" s="78"/>
       <c r="P25" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C25,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q25" s="78"/>
       <c r="R25" s="78"/>
@@ -10890,7 +10893,7 @@
       <c r="O26" s="78"/>
       <c r="P26" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C26,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q26" s="78"/>
       <c r="R26" s="78"/>
@@ -10940,7 +10943,7 @@
       <c r="O27" s="78"/>
       <c r="P27" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C27,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q27" s="78"/>
       <c r="R27" s="78"/>
@@ -10990,7 +10993,7 @@
       <c r="O28" s="78"/>
       <c r="P28" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C28,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q28" s="78"/>
       <c r="R28" s="78"/>
@@ -11040,7 +11043,7 @@
       <c r="O29" s="78"/>
       <c r="P29" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C29,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q29" s="78"/>
       <c r="R29" s="78"/>
@@ -11090,7 +11093,7 @@
       <c r="O30" s="78"/>
       <c r="P30" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C30,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q30" s="78"/>
       <c r="R30" s="78"/>
@@ -11140,7 +11143,7 @@
       <c r="O31" s="78"/>
       <c r="P31" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C31,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q31" s="78"/>
       <c r="R31" s="78"/>
@@ -11190,7 +11193,7 @@
       <c r="O32" s="78"/>
       <c r="P32" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C32,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q32" s="78"/>
       <c r="R32" s="78"/>
@@ -13389,7 +13392,7 @@
       </c>
       <c r="P73" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C73,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</v>
+        <v>**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</v>
       </c>
       <c r="Q73" s="56" t="s">
         <v>241</v>
@@ -13453,7 +13456,7 @@
       </c>
       <c r="P74" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C74,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</v>
+        <v>**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</v>
       </c>
       <c r="Q74" s="61" t="str">
         <f t="shared" si="15"/>
@@ -13519,7 +13522,7 @@
       </c>
       <c r="P75" s="191" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C75,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</v>
+        <v>**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Rural Residential:** In the BAU case, the share of electricity among fuels used by rural, residential buildings will rise from 39% to 42% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 64% by 2050. // **Commercial:** In the BAU case, the share of electricity among fuels used by commercial buildings will remain constant at 43% from 2017-2050 in the BAU case.  Setting this lever to 50% (of new sales in 2050) would likely result in the share of electricity used reaching 68% by 2050.</v>
       </c>
       <c r="Q75" s="61" t="str">
         <f t="shared" si="15"/>
@@ -31997,13 +32000,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="196" t="s">
@@ -32072,13 +32075,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" s="192" t="s">
+      <c r="A60" s="195" t="s">
         <v>200</v>
       </c>
-      <c r="B60" s="192"/>
-      <c r="C60" s="192"/>
-      <c r="D60" s="192"/>
-      <c r="E60" s="192"/>
+      <c r="B60" s="195"/>
+      <c r="C60" s="195"/>
+      <c r="D60" s="195"/>
+      <c r="E60" s="195"/>
     </row>
     <row r="85" spans="1:39" s="13" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="10" t="s">
@@ -32183,13 +32186,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.75">
-      <c r="A89" s="192" t="s">
+      <c r="A89" s="195" t="s">
         <v>201</v>
       </c>
-      <c r="B89" s="192"/>
-      <c r="C89" s="192"/>
-      <c r="D89" s="192"/>
-      <c r="E89" s="192"/>
+      <c r="B89" s="195"/>
+      <c r="C89" s="195"/>
+      <c r="D89" s="195"/>
+      <c r="E89" s="195"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.75">
       <c r="A90" s="10">
@@ -32276,13 +32279,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A98" s="192" t="s">
+      <c r="A98" s="195" t="s">
         <v>202</v>
       </c>
-      <c r="B98" s="192"/>
-      <c r="C98" s="192"/>
-      <c r="D98" s="192"/>
-      <c r="E98" s="192"/>
+      <c r="B98" s="195"/>
+      <c r="C98" s="195"/>
+      <c r="D98" s="195"/>
+      <c r="E98" s="195"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" s="18">
@@ -32366,13 +32369,13 @@
       <c r="A108" s="21"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A109" s="192" t="s">
+      <c r="A109" s="195" t="s">
         <v>204</v>
       </c>
-      <c r="B109" s="192"/>
-      <c r="C109" s="192"/>
-      <c r="D109" s="192"/>
-      <c r="E109" s="192"/>
+      <c r="B109" s="195"/>
+      <c r="C109" s="195"/>
+      <c r="D109" s="195"/>
+      <c r="E109" s="195"/>
     </row>
     <row r="110" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="111" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -32385,13 +32388,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A113" s="192" t="s">
+      <c r="A113" s="195" t="s">
         <v>203</v>
       </c>
-      <c r="B113" s="192"/>
-      <c r="C113" s="192"/>
-      <c r="D113" s="192"/>
-      <c r="E113" s="192"/>
+      <c r="B113" s="195"/>
+      <c r="C113" s="195"/>
+      <c r="D113" s="195"/>
+      <c r="E113" s="195"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A114" s="18">
@@ -32472,13 +32475,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A124" s="192" t="s">
+      <c r="A124" s="195" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="192"/>
-      <c r="C124" s="192"/>
-      <c r="D124" s="192"/>
-      <c r="E124" s="192"/>
+      <c r="B124" s="195"/>
+      <c r="C124" s="195"/>
+      <c r="D124" s="195"/>
+      <c r="E124" s="195"/>
       <c r="L124" s="22"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.75">
@@ -32569,13 +32572,13 @@
       <c r="C133" s="16"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A134" s="192" t="s">
+      <c r="A134" s="195" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="192"/>
-      <c r="C134" s="192"/>
-      <c r="D134" s="192"/>
-      <c r="E134" s="192"/>
+      <c r="B134" s="195"/>
+      <c r="C134" s="195"/>
+      <c r="D134" s="195"/>
+      <c r="E134" s="195"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A135" s="28" t="s">
@@ -32590,25 +32593,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A136" s="30"/>
-      <c r="B136" s="193" t="s">
+      <c r="B136" s="192" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="194"/>
-      <c r="D136" s="194"/>
-      <c r="E136" s="195"/>
+      <c r="C136" s="193"/>
+      <c r="D136" s="193"/>
+      <c r="E136" s="194"/>
       <c r="F136" s="29"/>
       <c r="G136" s="29"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A137" s="31"/>
-      <c r="B137" s="193" t="s">
+      <c r="B137" s="192" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="195"/>
-      <c r="D137" s="193" t="s">
+      <c r="C137" s="194"/>
+      <c r="D137" s="192" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="195"/>
+      <c r="E137" s="194"/>
       <c r="F137" s="29"/>
       <c r="G137" s="29"/>
     </row>
@@ -33155,13 +33158,13 @@
       <c r="G163" s="29"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A165" s="192" t="s">
+      <c r="A165" s="195" t="s">
         <v>207</v>
       </c>
-      <c r="B165" s="192"/>
-      <c r="C165" s="192"/>
-      <c r="D165" s="192"/>
-      <c r="E165" s="192"/>
+      <c r="B165" s="195"/>
+      <c r="C165" s="195"/>
+      <c r="D165" s="195"/>
+      <c r="E165" s="195"/>
     </row>
     <row r="166" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A166" s="24" t="s">
@@ -33184,10 +33187,10 @@
       <c r="B168" s="47"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A169" s="192" t="s">
+      <c r="A169" s="195" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="192"/>
+      <c r="B169" s="195"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" s="24" t="s">
@@ -33219,13 +33222,13 @@
       <c r="B173" s="47"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A174" s="192" t="s">
+      <c r="A174" s="195" t="s">
         <v>217</v>
       </c>
-      <c r="B174" s="192"/>
-      <c r="C174" s="192"/>
-      <c r="D174" s="192"/>
-      <c r="E174" s="192"/>
+      <c r="B174" s="195"/>
+      <c r="C174" s="195"/>
+      <c r="D174" s="195"/>
+      <c r="E174" s="195"/>
     </row>
     <row r="175" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A175" s="24" t="s">
@@ -33245,13 +33248,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A178" s="192" t="s">
+      <c r="A178" s="195" t="s">
         <v>210</v>
       </c>
-      <c r="B178" s="192"/>
-      <c r="C178" s="192"/>
-      <c r="D178" s="192"/>
-      <c r="E178" s="192"/>
+      <c r="B178" s="195"/>
+      <c r="C178" s="195"/>
+      <c r="D178" s="195"/>
+      <c r="E178" s="195"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" s="26" t="s">
@@ -33279,13 +33282,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A183" s="192" t="s">
+      <c r="A183" s="195" t="s">
         <v>212</v>
       </c>
-      <c r="B183" s="192"/>
-      <c r="C183" s="192"/>
-      <c r="D183" s="192"/>
-      <c r="E183" s="192"/>
+      <c r="B183" s="195"/>
+      <c r="C183" s="195"/>
+      <c r="D183" s="195"/>
+      <c r="E183" s="195"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" s="24" t="s">
@@ -33340,13 +33343,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A191" s="192" t="s">
+      <c r="A191" s="195" t="s">
         <v>228</v>
       </c>
-      <c r="B191" s="192"/>
-      <c r="C191" s="192"/>
-      <c r="D191" s="192"/>
-      <c r="E191" s="192"/>
+      <c r="B191" s="195"/>
+      <c r="C191" s="195"/>
+      <c r="D191" s="195"/>
+      <c r="E191" s="195"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" s="22" t="s">
@@ -33406,6 +33409,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -33420,12 +33429,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>